<commit_message>
remove customer module and made easy step to export
</commit_message>
<xml_diff>
--- a/public/mayurbhai_bhikhubhai_gajanotar.xlsx
+++ b/public/mayurbhai_bhikhubhai_gajanotar.xlsx
@@ -15,42 +15,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
-  <si>
-    <t>ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+  <si>
+    <t>Sr. No</t>
+  </si>
+  <si>
+    <t>Loan Account Number</t>
+  </si>
+  <si>
+    <t>Cust Id</t>
+  </si>
+  <si>
+    <t>Cust CIF</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Product</t>
   </si>
   <si>
     <t>EMI</t>
   </si>
   <si>
+    <t>POS</t>
+  </si>
+  <si>
     <t>Loan Amount</t>
   </si>
   <si>
-    <t>POS</t>
-  </si>
-  <si>
-    <t>15,000.00</t>
-  </si>
-  <si>
-    <t>125,000.00</t>
-  </si>
-  <si>
-    <t>12,000.00</t>
-  </si>
-  <si>
-    <t>13,000.00</t>
-  </si>
-  <si>
-    <t>16,000.00</t>
-  </si>
-  <si>
-    <t>18,000.00</t>
-  </si>
-  <si>
-    <t>19,000.00</t>
-  </si>
-  <si>
-    <t>370,000.00</t>
+    <t>Pennanent Address</t>
+  </si>
+  <si>
+    <t>Permanent Address</t>
+  </si>
+  <si>
+    <t>Communication Address</t>
+  </si>
+  <si>
+    <t>Pincode</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Email ID</t>
+  </si>
+  <si>
+    <t>Mobile No 1</t>
+  </si>
+  <si>
+    <t>Mobile No 2</t>
+  </si>
+  <si>
+    <t>Lok Adalat YES/ NO</t>
+  </si>
+  <si>
+    <t>Advocate</t>
+  </si>
+  <si>
+    <t>Court Location</t>
+  </si>
+  <si>
+    <t>CM/ACM/RCM Name</t>
+  </si>
+  <si>
+    <t>Contact No</t>
+  </si>
+  <si>
+    <t>MAYURBHAI BHIKHUBHAI GAJANOTAR</t>
+  </si>
+  <si>
+    <t>EMBEDDED FINANCE</t>
+  </si>
+  <si>
+    <t>₹15,000.00</t>
+  </si>
+  <si>
+    <t>C 1 304 WHITE PALACE VARIAV VATSALYA VILLA VARIAV SURAT GUJARAT Surat GJ 394520</t>
+  </si>
+  <si>
+    <t>Surat</t>
+  </si>
+  <si>
+    <t>Gujarat</t>
+  </si>
+  <si>
+    <t>mayurgajanotar@gmail.com</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Adv Ajay Desai</t>
+  </si>
+  <si>
+    <t>Ahmedabad</t>
+  </si>
+  <si>
+    <t>Chaudhari Lalitbhai</t>
+  </si>
+  <si>
+    <t>₹125,000.00</t>
+  </si>
+  <si>
+    <t>₹12,000.00</t>
+  </si>
+  <si>
+    <t>₹13,000.00</t>
+  </si>
+  <si>
+    <t>₹16,000.00</t>
+  </si>
+  <si>
+    <t>₹18,000.00</t>
+  </si>
+  <si>
+    <t>₹19,000.00</t>
+  </si>
+  <si>
+    <t>₹370,000.00</t>
   </si>
 </sst>
 </file>
@@ -58,7 +148,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -68,13 +158,28 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFefefef"/>
+        <bgColor rgb="FFefefef"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -89,8 +194,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,171 +498,857 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1:X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="11.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="27.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="12.568" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="9.998" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="36.42" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="19.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="7.427" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="7.427" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="17.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="25.422" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="94.263" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="94.263" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="12.568" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="8.855" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="9.998" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="29.421" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="17.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="17.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="26.708" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="22" max="22" width="21.566" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="24" max="24" width="16.425" bestFit="true" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:24">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:24">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>10542139</v>
+      </c>
+      <c r="C2">
+        <v>103103</v>
+      </c>
+      <c r="D2">
+        <v>103377</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2">
         <v>1408</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
+      <c r="I2">
         <v>7983</v>
       </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2">
+        <v>394520</v>
+      </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2">
+        <v>7359095117</v>
+      </c>
+      <c r="S2">
+        <v>7359095117</v>
+      </c>
+      <c r="T2" t="s">
+        <v>31</v>
+      </c>
+      <c r="U2" t="s">
+        <v>32</v>
+      </c>
+      <c r="V2" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2">
+        <v>9925120112</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:24">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
+        <v>6003414</v>
+      </c>
+      <c r="C3">
+        <v>103103</v>
+      </c>
+      <c r="D3">
+        <v>103377</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3">
         <v>3745</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
+      <c r="I3">
         <v>94941</v>
       </c>
+      <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3">
+        <v>394520</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3">
+        <v>7359095117</v>
+      </c>
+      <c r="S3">
+        <v>7359095117</v>
+      </c>
+      <c r="T3" t="s">
+        <v>31</v>
+      </c>
+      <c r="U3" t="s">
+        <v>32</v>
+      </c>
+      <c r="V3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3">
+        <v>9925120112</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:24">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>9192496</v>
+      </c>
+      <c r="C4">
+        <v>103103</v>
+      </c>
+      <c r="D4">
+        <v>103377</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4">
         <v>1123</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
+      <c r="I4">
         <v>3343</v>
       </c>
+      <c r="J4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4">
+        <v>394520</v>
+      </c>
+      <c r="O4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4">
+        <v>7359095117</v>
+      </c>
+      <c r="S4">
+        <v>7359095117</v>
+      </c>
+      <c r="T4" t="s">
+        <v>31</v>
+      </c>
+      <c r="U4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V4" t="s">
+        <v>33</v>
+      </c>
+      <c r="W4" t="s">
+        <v>34</v>
+      </c>
+      <c r="X4">
+        <v>9925120112</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:24">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
+        <v>9596239</v>
+      </c>
+      <c r="C5">
+        <v>103103</v>
+      </c>
+      <c r="D5">
+        <v>103377</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5">
         <v>1123</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
+      <c r="I5">
         <v>4338</v>
       </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5">
+        <v>394520</v>
+      </c>
+      <c r="O5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5">
+        <v>7359095117</v>
+      </c>
+      <c r="S5">
+        <v>7359095117</v>
+      </c>
+      <c r="T5" t="s">
+        <v>31</v>
+      </c>
+      <c r="U5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V5" t="s">
+        <v>33</v>
+      </c>
+      <c r="W5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X5">
+        <v>9925120112</v>
+      </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:24">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
+        <v>9800562</v>
+      </c>
+      <c r="C6">
+        <v>103103</v>
+      </c>
+      <c r="D6">
+        <v>103377</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6">
         <v>1217</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6">
+      <c r="I6">
         <v>4585</v>
       </c>
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6">
+        <v>394520</v>
+      </c>
+      <c r="O6" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>30</v>
+      </c>
+      <c r="R6">
+        <v>7359095117</v>
+      </c>
+      <c r="S6">
+        <v>7359095117</v>
+      </c>
+      <c r="T6" t="s">
+        <v>31</v>
+      </c>
+      <c r="U6" t="s">
+        <v>32</v>
+      </c>
+      <c r="V6" t="s">
+        <v>33</v>
+      </c>
+      <c r="W6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X6">
+        <v>9925120112</v>
+      </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:24">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
+        <v>10525983</v>
+      </c>
+      <c r="C7">
+        <v>103103</v>
+      </c>
+      <c r="D7">
+        <v>103377</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7">
         <v>1408</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7">
+      <c r="I7">
         <v>9269</v>
       </c>
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7">
+        <v>394520</v>
+      </c>
+      <c r="O7" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R7">
+        <v>7359095117</v>
+      </c>
+      <c r="S7">
+        <v>7359095117</v>
+      </c>
+      <c r="T7" t="s">
+        <v>31</v>
+      </c>
+      <c r="U7" t="s">
+        <v>32</v>
+      </c>
+      <c r="V7" t="s">
+        <v>33</v>
+      </c>
+      <c r="W7" t="s">
+        <v>34</v>
+      </c>
+      <c r="X7">
+        <v>9925120112</v>
+      </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:24">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
+        <v>10911879</v>
+      </c>
+      <c r="C8">
+        <v>103103</v>
+      </c>
+      <c r="D8">
+        <v>103377</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8">
         <v>1501</v>
       </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8">
+      <c r="I8">
         <v>11224</v>
       </c>
+      <c r="J8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8">
+        <v>394520</v>
+      </c>
+      <c r="O8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>30</v>
+      </c>
+      <c r="R8">
+        <v>7359095117</v>
+      </c>
+      <c r="S8">
+        <v>7359095117</v>
+      </c>
+      <c r="T8" t="s">
+        <v>31</v>
+      </c>
+      <c r="U8" t="s">
+        <v>32</v>
+      </c>
+      <c r="V8" t="s">
+        <v>33</v>
+      </c>
+      <c r="W8" t="s">
+        <v>34</v>
+      </c>
+      <c r="X8">
+        <v>9925120112</v>
+      </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:24">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
+        <v>11326502</v>
+      </c>
+      <c r="C9">
+        <v>103103</v>
+      </c>
+      <c r="D9">
+        <v>103377</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9">
         <v>1707</v>
       </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9">
+      <c r="I9">
         <v>14059</v>
       </c>
+      <c r="J9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9">
+        <v>394520</v>
+      </c>
+      <c r="O9" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>30</v>
+      </c>
+      <c r="R9">
+        <v>7359095117</v>
+      </c>
+      <c r="S9">
+        <v>7359095117</v>
+      </c>
+      <c r="T9" t="s">
+        <v>31</v>
+      </c>
+      <c r="U9" t="s">
+        <v>32</v>
+      </c>
+      <c r="V9" t="s">
+        <v>33</v>
+      </c>
+      <c r="W9" t="s">
+        <v>34</v>
+      </c>
+      <c r="X9">
+        <v>9925120112</v>
+      </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:24">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
+        <v>11619811</v>
+      </c>
+      <c r="C10">
+        <v>103103</v>
+      </c>
+      <c r="D10">
+        <v>103377</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10">
         <v>1801</v>
       </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10">
+      <c r="I10">
         <v>16403</v>
       </c>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10">
+        <v>394520</v>
+      </c>
+      <c r="O10" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>30</v>
+      </c>
+      <c r="R10">
+        <v>7359095117</v>
+      </c>
+      <c r="S10">
+        <v>7359095117</v>
+      </c>
+      <c r="T10" t="s">
+        <v>31</v>
+      </c>
+      <c r="U10" t="s">
+        <v>32</v>
+      </c>
+      <c r="V10" t="s">
+        <v>33</v>
+      </c>
+      <c r="W10" t="s">
+        <v>34</v>
+      </c>
+      <c r="X10">
+        <v>9925120112</v>
+      </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:24">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
+        <v>5592552</v>
+      </c>
+      <c r="C11">
+        <v>103103</v>
+      </c>
+      <c r="D11">
+        <v>103377</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11">
         <v>4113</v>
       </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11">
+      <c r="I11">
         <v>88581</v>
       </c>
+      <c r="J11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N11">
+        <v>394520</v>
+      </c>
+      <c r="O11" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>30</v>
+      </c>
+      <c r="R11">
+        <v>7359095117</v>
+      </c>
+      <c r="S11">
+        <v>7359095117</v>
+      </c>
+      <c r="T11" t="s">
+        <v>31</v>
+      </c>
+      <c r="U11" t="s">
+        <v>32</v>
+      </c>
+      <c r="V11" t="s">
+        <v>33</v>
+      </c>
+      <c r="W11" t="s">
+        <v>34</v>
+      </c>
+      <c r="X11">
+        <v>9925120112</v>
+      </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="C12" t="s">
-        <v>11</v>
+    <row r="12" spans="1:24">
+      <c r="J12" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>